<commit_message>
Integrated Order Search, PriceInquiry and Email Send Options
</commit_message>
<xml_diff>
--- a/Dimension/TestData/TestData.xlsx
+++ b/Dimension/TestData/TestData.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lt\eclipse-workspace\Dimension\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lt\git\Dimension\Dimension\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE09AB46-1DA7-46E0-9391-9F9FF806610D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74CA889-191E-4C9A-B506-35AC1362E1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4F066510-B6C8-4948-B76B-550790CE6937}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4F066510-B6C8-4948-B76B-550790CE6937}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="WorkCenter_Order" sheetId="3" r:id="rId2"/>
-    <sheet name="SubContractor" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
-    <sheet name="MyProfile" sheetId="2" r:id="rId5"/>
+    <sheet name="LoginVerify" sheetId="5" r:id="rId2"/>
+    <sheet name="WorkCenter_Order" sheetId="3" r:id="rId3"/>
+    <sheet name="PrinceInquiryData" sheetId="6" r:id="rId4"/>
+    <sheet name="Mail" sheetId="7" r:id="rId5"/>
+    <sheet name="SubContractor" sheetId="4" r:id="rId6"/>
+    <sheet name="MyProfile" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>UserName</t>
   </si>
@@ -89,6 +90,12 @@
   </si>
   <si>
     <t>Sub Contractor</t>
+  </si>
+  <si>
+    <t>MailID</t>
+  </si>
+  <si>
+    <t>lthiyagaraj@speedstep.de</t>
   </si>
 </sst>
 </file>
@@ -474,7 +481,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,11 +521,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970DE5F7-8E01-47E4-921B-C4FD7DF19BCF}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{1A1B4B21-B7C2-4A46-9EAA-7B7554FBD0E3}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{6347BB99-9654-466B-AF95-8F1FC9655BDC}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{7AFA5BEC-1DA3-4103-A54C-7E76928A207F}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{8C13A9BE-806A-4101-BDE5-BFBF2723675A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526E9561-972C-4AC1-AB83-C2C8A69097C1}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,11 +635,78 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE395D43-B8F2-4D63-B3E0-2593D802FBBB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2071759</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960BE32E-D37F-4480-A2E0-3052BAB4102A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8E158A95-E0B9-44FD-AC9E-AF57A2457507}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B4B886-CD50-45B3-8648-C9965B357F38}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -575,60 +730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970DE5F7-8E01-47E4-921B-C4FD7DF19BCF}">
-  <dimension ref="G23:I25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:K25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G23" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G25" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H24" r:id="rId1" xr:uid="{1A1B4B21-B7C2-4A46-9EAA-7B7554FBD0E3}"/>
-    <hyperlink ref="H25" r:id="rId2" xr:uid="{6347BB99-9654-466B-AF95-8F1FC9655BDC}"/>
-    <hyperlink ref="H23" r:id="rId3" xr:uid="{7AFA5BEC-1DA3-4103-A54C-7E76928A207F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2399A19B-1575-4287-A85B-49029B89EF78}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Login Invalid User and Already Login scenarios handled. Price Inquiry modules added
</commit_message>
<xml_diff>
--- a/Dimension/TestData/TestData.xlsx
+++ b/Dimension/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lt\git\Dimension\Dimension\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74CA889-191E-4C9A-B506-35AC1362E1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ACD1DC-A35D-4B3C-896F-7542AC2E3F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4F066510-B6C8-4948-B76B-550790CE6937}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F066510-B6C8-4948-B76B-550790CE6937}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24F048D-8714-4694-B0E1-C6D0B64EE851}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960BE32E-D37F-4480-A2E0-3052BAB4102A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>